<commit_message>
Updated spreadsheet & schematic
Added the following/
- Added chosen diode and op amp for components spreadsheet
- Created schematic file in KiCad
- Updated KiCad component library with added diode and op amp
</commit_message>
<xml_diff>
--- a/Circuit_Components.xlsx
+++ b/Circuit_Components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\EEG-Individual-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JZ\Documents\GitHub\EEG-Individual-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF9D2FA-9872-4D0D-8B0A-FC8FD361586A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8E42ED-EFF3-42F7-A2AE-B77072F95AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15460" xr2:uid="{8AEB05BA-5260-4D6C-B715-5CE7F81457BA}"/>
+    <workbookView xWindow="0" yWindow="1980" windowWidth="17280" windowHeight="8964" xr2:uid="{8AEB05BA-5260-4D6C-B715-5CE7F81457BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Instrumentation amplifier</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>OPA172IDR</t>
+  </si>
+  <si>
+    <t>SP4203-01FTG-C</t>
   </si>
 </sst>
 </file>
@@ -557,21 +560,21 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -594,12 +597,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -621,10 +624,10 @@
       </c>
       <c r="I3" s="4">
         <f>SUM(G3:G55)</f>
-        <v>25.849999999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>41.209999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -645,7 +648,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -663,13 +666,13 @@
         <v>10.83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -690,7 +693,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -711,7 +714,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -732,7 +735,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -753,7 +756,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -763,18 +766,21 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11" s="4">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -795,7 +801,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -816,7 +822,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -837,25 +843,31 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>15</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16" s="4">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -876,7 +888,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -897,19 +909,25 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E20">
         <v>1</v>
       </c>
+      <c r="F20" s="4">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G20" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -918,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -939,7 +957,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -960,7 +978,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -981,27 +999,31 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="4">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -1022,25 +1044,31 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>15</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E28">
         <v>1</v>
       </c>
+      <c r="F28" s="4">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="G28" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1061,7 +1089,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1078,11 +1106,11 @@
         <v>1.18</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" ref="G31:G32" si="1">E31*F31</f>
+        <f t="shared" ref="G31:G34" si="1">E31*F31</f>
         <v>1.18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>7</v>
       </c>
@@ -1103,17 +1131,28 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>41</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E34">
         <v>4</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="1"/>
+        <v>3.96</v>
       </c>
     </row>
   </sheetData>
@@ -1138,8 +1177,13 @@
     <hyperlink ref="D31" r:id="rId18" display="https://www.digikey.com.au/en/products/detail/panasonic-electronic-components/ECH-U1H333JX5/340777" xr:uid="{91416F90-484A-48A6-BCB4-309340305239}"/>
     <hyperlink ref="D32" r:id="rId19" display="https://www.digikey.com.au/en/products/detail/koa-speer-electronics-inc/RN73H1JTTD4991B25/10678570" xr:uid="{9F0926F7-E6F6-440B-9685-9D038BBE703F}"/>
     <hyperlink ref="D11" r:id="rId20" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{3FC86F97-A9D2-4073-9A22-84D7DE1246E9}"/>
+    <hyperlink ref="D16" r:id="rId21" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{0F129D8A-CD30-4B12-9503-63D4AC9ABE45}"/>
+    <hyperlink ref="D20" r:id="rId22" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{83D7D604-468F-48F7-9338-64F7A6082A58}"/>
+    <hyperlink ref="D25" r:id="rId23" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{10EB80B0-ED9E-4A48-A8A1-34B5520C5E34}"/>
+    <hyperlink ref="D28" r:id="rId24" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{C170AB32-1EAC-4907-B60E-7E609112428C}"/>
+    <hyperlink ref="D34" r:id="rId25" display="https://www.digikey.com.au/en/products/detail/littelfuse-inc/SP4203-01FTG-C/9828985" xr:uid="{2FDC177B-652A-4C0F-929D-B89F51A6A216}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated KiCad project schematic & symbol library
Changed diode choice to D5V0F1U2S9-7
Total cost currently $39.85
</commit_message>
<xml_diff>
--- a/Circuit_Components.xlsx
+++ b/Circuit_Components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JZ\Documents\GitHub\EEG-Individual-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\EEG-Individual-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8E42ED-EFF3-42F7-A2AE-B77072F95AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8D9CF1-79EE-47C1-A3DD-149D7DFF062E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1980" windowWidth="17280" windowHeight="8964" xr2:uid="{8AEB05BA-5260-4D6C-B715-5CE7F81457BA}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15460" xr2:uid="{8AEB05BA-5260-4D6C-B715-5CE7F81457BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
     <t>OPA172IDR</t>
   </si>
   <si>
-    <t>SP4203-01FTG-C</t>
+    <t>D5V0F1U2S9-7</t>
   </si>
 </sst>
 </file>
@@ -560,21 +560,21 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -597,12 +597,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -624,10 +624,10 @@
       </c>
       <c r="I3" s="4">
         <f>SUM(G3:G55)</f>
-        <v>41.209999999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>39.849999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -648,7 +648,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -666,13 +666,13 @@
         <v>10.83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -714,7 +714,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -756,7 +756,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -774,13 +774,13 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -801,7 +801,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -843,7 +843,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -861,13 +861,13 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -888,7 +888,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -927,7 +927,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -957,7 +957,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -978,7 +978,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -999,7 +999,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>15</v>
       </c>
@@ -1017,13 +1017,13 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>15</v>
       </c>
@@ -1062,13 +1062,13 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>7</v>
       </c>
@@ -1131,13 +1131,13 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>41</v>
       </c>
@@ -1148,11 +1148,11 @@
         <v>4</v>
       </c>
       <c r="F34" s="4">
-        <v>0.99</v>
+        <v>0.65</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="1"/>
-        <v>3.96</v>
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1181,7 @@
     <hyperlink ref="D20" r:id="rId22" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{83D7D604-468F-48F7-9338-64F7A6082A58}"/>
     <hyperlink ref="D25" r:id="rId23" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{10EB80B0-ED9E-4A48-A8A1-34B5520C5E34}"/>
     <hyperlink ref="D28" r:id="rId24" display="https://www.digikey.com.au/en/products/detail/texas-instruments/OPA172IDR/4695363" xr:uid="{C170AB32-1EAC-4907-B60E-7E609112428C}"/>
-    <hyperlink ref="D34" r:id="rId25" display="https://www.digikey.com.au/en/products/detail/littelfuse-inc/SP4203-01FTG-C/9828985" xr:uid="{2FDC177B-652A-4C0F-929D-B89F51A6A216}"/>
+    <hyperlink ref="D34" r:id="rId25" display="https://www.digikey.com.au/en/products/detail/diodes-incorporated/D5V0F1U2S9-7/4967035" xr:uid="{E2ADF663-F86B-4975-9D20-2ACE01A65256}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId26"/>

</xml_diff>